<commit_message>
pushing updated date for the winter data
</commit_message>
<xml_diff>
--- a/avbernat_working_on/stats/data/demographic_data_winter2020-coors.corrected.xlsx
+++ b/avbernat_working_on/stats/data/demographic_data_winter2020-coors.corrected.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10307"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anastasiabernat/Desktop/Rstats-winter2020/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anastasiabernat/Desktop/Rstats-winter2020/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A7DC596-99C0-944B-8405-F063D0B3682C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD82758D-BD82-E04F-8547-EAD6E809955C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3060" yWindow="460" windowWidth="19340" windowHeight="16660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -425,8 +425,8 @@
   <dimension ref="A1:I1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A248" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B254" sqref="B254"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1886,7 +1886,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
update to the yes-no script because of the 1 typo
</commit_message>
<xml_diff>
--- a/avbernat_working_on/stats/data/demographic_data_winter2020-coors.corrected.xlsx
+++ b/avbernat_working_on/stats/data/demographic_data_winter2020-coors.corrected.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anastasiabernat/Desktop/Rstats-winter2020/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD82758D-BD82-E04F-8547-EAD6E809955C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13A676CE-19B1-864A-B474-545F6C1FCCF9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3060" yWindow="460" windowWidth="19340" windowHeight="16660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -425,8 +425,8 @@
   <dimension ref="A1:I1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B51" sqref="B51"/>
+      <pane ySplit="1" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C102" sqref="C102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3536,7 +3536,7 @@
         <v>103</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C104" s="2" t="s">
         <v>9</v>

</xml_diff>